<commit_message>
Mobile synch and db changes
</commit_message>
<xml_diff>
--- a/data/db.xlsx
+++ b/data/db.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="242">
   <si>
     <t>field</t>
   </si>
@@ -714,13 +714,34 @@
     <t>27844801653</t>
   </si>
   <si>
-    <t>mobile_content</t>
-  </si>
-  <si>
     <t>html</t>
   </si>
   <si>
     <t>js</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>home</t>
+  </si>
+  <si>
+    <t>settings</t>
+  </si>
+  <si>
+    <t>Hi, this is the home page!</t>
+  </si>
+  <si>
+    <t>Hi! Setting page here :)</t>
+  </si>
+  <si>
+    <t>2013-03-16 19:30:00</t>
+  </si>
+  <si>
+    <t>alert("home page loaded");</t>
+  </si>
+  <si>
+    <t>alert("settings page loaded");</t>
   </si>
 </sst>
 </file>
@@ -1086,7 +1107,7 @@
   <dimension ref="A1:T206"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,9 +1115,7 @@
     <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.140625" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="86.28515625" customWidth="1"/>
-    <col min="6" max="10" width="17" customWidth="1"/>
+    <col min="4" max="10" width="4.85546875" customWidth="1"/>
     <col min="11" max="11" width="17" style="4" customWidth="1"/>
     <col min="12" max="16" width="21.140625" style="4" customWidth="1"/>
     <col min="17" max="20" width="13.28515625" style="4" customWidth="1"/>
@@ -1166,7 +1185,7 @@
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>232</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -1179,6 +1198,12 @@
       </c>
       <c r="F3">
         <v>1</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -1194,10 +1219,16 @@
       <c r="F4">
         <v>1</v>
       </c>
+      <c r="K4" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
@@ -1205,16 +1236,28 @@
       <c r="F5">
         <v>0</v>
       </c>
+      <c r="K5" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
       </c>
       <c r="F6">
         <v>0</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
@@ -1227,6 +1270,12 @@
       <c r="F7">
         <v>1</v>
       </c>
+      <c r="K7" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -1238,6 +1287,12 @@
       <c r="F8">
         <v>0</v>
       </c>
+      <c r="K8" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -1254,6 +1309,12 @@
       </c>
       <c r="G9">
         <v>0</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>